<commit_message>
Updates to data structure
</commit_message>
<xml_diff>
--- a/data/figure-data.xlsx
+++ b/data/figure-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmor7802/repos/bivariate-map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C82FAB-CDA7-DA4A-A742-1E8679274975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92880A56-36E0-2649-8344-9BB9692B03F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="-19440" windowWidth="27160" windowHeight="16580" tabRatio="500" xr2:uid="{D0AE1AC3-FFDD-DB40-87A2-A3D733A83E2C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{D0AE1AC3-FFDD-DB40-87A2-A3D733A83E2C}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="9" r:id="rId1"/>
@@ -30,28 +30,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -976,7 +954,7 @@
   <dimension ref="A1:G205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G205" sqref="G2:G205"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1011,12 +989,10 @@
       <c r="C2">
         <v>19.399999999999999</v>
       </c>
-      <c r="D2" cm="1">
-        <f t="array" ref="D2:D168">IF(B2:B168&gt;0,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E2" cm="1">
-        <f t="array" ref="E2:E168">IF(A2:A168&gt;0,1,0)</f>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
       <c r="G2" s="7"/>
@@ -1221,16 +1197,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="B14">
-        <v>61.501597444089462</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>5.4</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1239,16 +1215,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B15">
-        <v>85.112936344969199</v>
+        <v>0</v>
       </c>
       <c r="C15">
         <v>9.8000000000000007</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1257,10 +1233,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>169</v>
+        <v>108</v>
       </c>
       <c r="B16">
-        <v>70.314505776636722</v>
+        <v>61.501597444089462</v>
       </c>
       <c r="C16">
         <v>20.100000000000001</v>
@@ -1275,10 +1251,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="B17">
-        <v>48.954286186657846</v>
+        <v>85.112936344969199</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1293,10 +1269,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>169</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>70.314505776636722</v>
       </c>
       <c r="C18">
         <v>22</v>
@@ -1311,10 +1287,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>120</v>
+        <v>12</v>
       </c>
       <c r="B19">
-        <v>100</v>
+        <v>48.954286186657846</v>
       </c>
       <c r="C19">
         <v>3.5</v>
@@ -1329,10 +1305,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20">
-        <v>66.666666666666657</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>4.8</v>
@@ -1347,16 +1323,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C21">
         <v>15.1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1365,16 +1341,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>139</v>
+        <v>14</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1437,16 +1413,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="B26">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1455,10 +1431,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="B27">
-        <v>98.347107438016536</v>
+        <v>100</v>
       </c>
       <c r="C27">
         <v>24.7</v>
@@ -1473,10 +1449,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>170</v>
       </c>
       <c r="B28">
-        <v>32.296756996890267</v>
+        <v>98.347107438016536</v>
       </c>
       <c r="C28">
         <v>25.1</v>
@@ -1491,10 +1467,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29">
-        <v>0.63184245947034967</v>
+        <v>32.296756996890267</v>
       </c>
       <c r="C29">
         <v>3.7</v>
@@ -1509,10 +1485,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>115</v>
+        <v>18</v>
       </c>
       <c r="B30">
-        <v>97.945707997065298</v>
+        <v>0.63184245947034967</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1527,13 +1503,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>115</v>
       </c>
       <c r="B31">
-        <v>99.006622516556291</v>
+        <v>97.945707997065298</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>4.7</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1545,13 +1521,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>122</v>
+        <v>19</v>
       </c>
       <c r="B32">
-        <v>100</v>
+        <v>99.006622516556291</v>
       </c>
       <c r="C32">
-        <v>4.7</v>
+        <v>11.3</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1569,7 +1545,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <v>11.3</v>
+        <v>17.3</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1581,16 +1557,16 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C34">
-        <v>17.3</v>
+        <v>40.5</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -1599,16 +1575,16 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="B35">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C35">
-        <v>40.5</v>
+        <v>3</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1617,13 +1593,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>123</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1635,16 +1611,16 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>142</v>
+        <v>20</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37">
-        <v>16.600000000000001</v>
+        <v>2.5</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -1653,16 +1629,16 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="B38">
-        <v>89.017341040462426</v>
+        <v>0</v>
       </c>
       <c r="C38">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -1671,13 +1647,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>89.017341040462426</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>3.6</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -1689,13 +1665,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B40">
-        <v>99.759615384615387</v>
+        <v>1</v>
       </c>
       <c r="C40">
-        <v>3.6</v>
+        <v>1</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1707,16 +1683,16 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>58.441558441558442</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>41.6</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -1725,16 +1701,16 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>98.469387755102048</v>
       </c>
       <c r="C42">
-        <v>41.6</v>
+        <v>29.6</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -1743,16 +1719,16 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>145</v>
+        <v>23</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43">
-        <v>29.6</v>
+        <v>1</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -1761,13 +1737,13 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -1779,16 +1755,16 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>114</v>
+        <v>144</v>
       </c>
       <c r="B45">
-        <v>58.441558441558442</v>
+        <v>0</v>
       </c>
       <c r="C45">
-        <v>19.899999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -1797,16 +1773,16 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>110</v>
+        <v>168</v>
       </c>
       <c r="B46">
-        <v>98.469387755102048</v>
+        <v>0</v>
       </c>
       <c r="C46">
-        <v>3.8</v>
+        <v>13.5</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -1815,16 +1791,16 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>23</v>
+        <v>146</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47">
-        <v>13.5</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -1833,16 +1809,16 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>146</v>
+        <v>24</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>99.130434782608702</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -1851,13 +1827,13 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B49">
-        <v>99.130434782608702</v>
+        <v>59.898420494502425</v>
       </c>
       <c r="C49">
-        <v>11.5</v>
+        <v>5.2</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1869,13 +1845,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="B50">
-        <v>59.898420494502425</v>
+        <v>100</v>
       </c>
       <c r="C50">
-        <v>5.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -1887,13 +1863,13 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>124</v>
+        <v>26</v>
       </c>
       <c r="B51">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C51">
-        <v>9.1999999999999993</v>
+        <v>1</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -1905,13 +1881,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -1923,13 +1899,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>135</v>
+        <v>27</v>
       </c>
       <c r="B53">
-        <v>100</v>
+        <v>37.980456026058633</v>
       </c>
       <c r="C53">
-        <v>21</v>
+        <v>21.9</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -1941,13 +1917,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>27</v>
+        <v>125</v>
       </c>
       <c r="B54">
-        <v>37.980456026058633</v>
+        <v>100</v>
       </c>
       <c r="C54">
-        <v>21.9</v>
+        <v>6.1</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -1959,13 +1935,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>125</v>
+        <v>28</v>
       </c>
       <c r="B55">
-        <v>100</v>
+        <v>11.165644171779141</v>
       </c>
       <c r="C55">
-        <v>6.1</v>
+        <v>1</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -1977,10 +1953,10 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B56">
-        <v>11.165644171779141</v>
+        <v>1</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -1995,16 +1971,16 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>29</v>
+        <v>147</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>4.5</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -2013,13 +1989,13 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B58">
         <v>0</v>
       </c>
       <c r="C58">
-        <v>4.5</v>
+        <v>14.1</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -2031,16 +2007,16 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>148</v>
+        <v>30</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>94.989561586638828</v>
       </c>
       <c r="C59">
-        <v>14.1</v>
+        <v>6.8</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -2049,13 +2025,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B60">
-        <v>94.989561586638828</v>
+        <v>1</v>
       </c>
       <c r="C60">
-        <v>6.8</v>
+        <v>1</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -2067,16 +2043,16 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>31</v>
+        <v>149</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -2085,16 +2061,16 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>149</v>
+        <v>32</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>26.607929515418505</v>
       </c>
       <c r="C62">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -2103,13 +2079,13 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B63">
-        <v>26.607929515418505</v>
+        <v>99.80952380952381</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>15.7</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -2121,13 +2097,13 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="B64">
-        <v>99.80952380952381</v>
+        <v>100</v>
       </c>
       <c r="C64">
-        <v>15.7</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -2139,16 +2115,16 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="B65">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C65">
-        <v>17.399999999999999</v>
+        <v>21</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -2157,13 +2133,13 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B66">
         <v>0</v>
       </c>
       <c r="C66">
-        <v>21</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -2175,16 +2151,16 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C67">
-        <v>8.6999999999999993</v>
+        <v>41.1</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -2193,13 +2169,13 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>127</v>
+        <v>34</v>
       </c>
       <c r="B68">
-        <v>100</v>
+        <v>99.672131147540995</v>
       </c>
       <c r="C68">
-        <v>41.1</v>
+        <v>15.9</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -2211,16 +2187,16 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>34</v>
+        <v>152</v>
       </c>
       <c r="B69">
-        <v>99.672131147540995</v>
+        <v>0</v>
       </c>
       <c r="C69">
-        <v>15.9</v>
+        <v>0</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -2235,7 +2211,7 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70">
         <v>1</v>
@@ -2247,7 +2223,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -2265,16 +2241,16 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>153</v>
+        <v>36</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>1.6055527424075882E-2</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>14.8</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -2283,13 +2259,13 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>36</v>
+        <v>128</v>
       </c>
       <c r="B73">
-        <v>1.6055527424075882E-2</v>
+        <v>99.278474488919429</v>
       </c>
       <c r="C73">
-        <v>14.8</v>
+        <v>13.1</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -2301,13 +2277,13 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="B74">
-        <v>99.278474488919429</v>
+        <v>11.556363636363637</v>
       </c>
       <c r="C74">
-        <v>13.1</v>
+        <v>7.5</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -2319,13 +2295,13 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="B75">
-        <v>11.556363636363637</v>
+        <v>54.674361088211043</v>
       </c>
       <c r="C75">
-        <v>7.5</v>
+        <v>13.7</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -2337,13 +2313,13 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B76">
-        <v>54.674361088211043</v>
+        <v>65.797546012269933</v>
       </c>
       <c r="C76">
-        <v>13.7</v>
+        <v>1</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -2355,10 +2331,10 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B77">
-        <v>65.797546012269933</v>
+        <v>94.199896426721907</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -2373,10 +2349,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B78">
-        <v>94.199896426721907</v>
+        <v>41.761771916476462</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -2391,16 +2367,16 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>40</v>
+        <v>154</v>
       </c>
       <c r="B79">
-        <v>41.761771916476462</v>
+        <v>0</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -2409,16 +2385,16 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>154</v>
+        <v>41</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>92.030096140448663</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -2427,13 +2403,13 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B81">
-        <v>92.030096140448663</v>
+        <v>97.371565113500608</v>
       </c>
       <c r="C81">
-        <v>3.2</v>
+        <v>6.2</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -2445,13 +2421,13 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B82">
-        <v>97.371565113500608</v>
+        <v>1</v>
       </c>
       <c r="C82">
-        <v>6.2</v>
+        <v>3.2</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -2463,13 +2439,13 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>64.907470870459221</v>
       </c>
       <c r="C83">
-        <v>3.2</v>
+        <v>21.7</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -2481,13 +2457,13 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B84">
-        <v>64.907470870459221</v>
+        <v>100</v>
       </c>
       <c r="C84">
-        <v>21.7</v>
+        <v>1</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -2499,13 +2475,13 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B85">
-        <v>100</v>
+        <v>36.185243328100469</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>7.4</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -2517,16 +2493,16 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>46</v>
+        <v>155</v>
       </c>
       <c r="B86">
-        <v>36.185243328100469</v>
+        <v>0</v>
       </c>
       <c r="C86">
-        <v>7.4</v>
+        <v>0</v>
       </c>
       <c r="D86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -2535,16 +2511,16 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>155</v>
+        <v>47</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -2553,13 +2529,13 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>86.129032258064512</v>
       </c>
       <c r="C88">
-        <v>1</v>
+        <v>5.5</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -2571,13 +2547,13 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B89">
-        <v>86.129032258064512</v>
+        <v>81.132075471698116</v>
       </c>
       <c r="C89">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -2589,13 +2565,13 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B90">
-        <v>81.132075471698116</v>
+        <v>93.24116743471582</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>6.6</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -2607,13 +2583,13 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B91">
-        <v>93.24116743471582</v>
+        <v>1</v>
       </c>
       <c r="C91">
-        <v>6.6</v>
+        <v>1</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -2625,10 +2601,10 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B92">
-        <v>1</v>
+        <v>13.541666666666666</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -2643,13 +2619,13 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B93">
-        <v>13.541666666666666</v>
+        <v>94.642857142857139</v>
       </c>
       <c r="C93">
-        <v>1</v>
+        <v>26.9</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -2661,13 +2637,13 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B94">
-        <v>94.642857142857139</v>
+        <v>98.843930635838149</v>
       </c>
       <c r="C94">
-        <v>26.9</v>
+        <v>13.6</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -2679,13 +2655,13 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="B95">
-        <v>98.843930635838149</v>
+        <v>98.439450686641692</v>
       </c>
       <c r="C95">
-        <v>13.6</v>
+        <v>3.5</v>
       </c>
       <c r="D95">
         <v>1</v>
@@ -2697,13 +2673,13 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>129</v>
+        <v>55</v>
       </c>
       <c r="B96">
-        <v>98.439450686641692</v>
+        <v>95.215311004784681</v>
       </c>
       <c r="C96">
-        <v>3.5</v>
+        <v>6.6</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -2715,13 +2691,13 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B97">
-        <v>95.215311004784681</v>
+        <v>83.116883116883116</v>
       </c>
       <c r="C97">
-        <v>6.6</v>
+        <v>1</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -2733,13 +2709,13 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B98">
-        <v>83.116883116883116</v>
+        <v>99.453551912568301</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -2751,16 +2727,16 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>57</v>
+        <v>156</v>
       </c>
       <c r="B99">
-        <v>99.453551912568301</v>
+        <v>0</v>
       </c>
       <c r="C99">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -2769,16 +2745,16 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>156</v>
+        <v>58</v>
       </c>
       <c r="B100">
-        <v>0</v>
+        <v>43.769775500979357</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -2787,13 +2763,13 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B101">
-        <v>43.769775500979357</v>
+        <v>31.411530815109344</v>
       </c>
       <c r="C101">
-        <v>4.0999999999999996</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="D101">
         <v>1</v>
@@ -2805,13 +2781,13 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B102">
-        <v>31.411530815109344</v>
+        <v>99.397590361445793</v>
       </c>
       <c r="C102">
-        <v>17.100000000000001</v>
+        <v>1</v>
       </c>
       <c r="D102">
         <v>1</v>
@@ -2823,13 +2799,13 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B103">
-        <v>99.397590361445793</v>
+        <v>49.334995843724023</v>
       </c>
       <c r="C103">
-        <v>1</v>
+        <v>4.8</v>
       </c>
       <c r="D103">
         <v>1</v>
@@ -2841,13 +2817,13 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B104">
-        <v>49.334995843724023</v>
+        <v>96.779964221824685</v>
       </c>
       <c r="C104">
-        <v>4.8</v>
+        <v>22.2</v>
       </c>
       <c r="D104">
         <v>1</v>
@@ -2859,13 +2835,13 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B105">
-        <v>96.779964221824685</v>
+        <v>55.086848635235732</v>
       </c>
       <c r="C105">
-        <v>22.2</v>
+        <v>11</v>
       </c>
       <c r="D105">
         <v>1</v>
@@ -2877,13 +2853,13 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B106">
-        <v>55.086848635235732</v>
+        <v>82.432432432432435</v>
       </c>
       <c r="C106">
-        <v>11</v>
+        <v>29.2</v>
       </c>
       <c r="D106">
         <v>1</v>
@@ -2895,13 +2871,13 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B107">
-        <v>82.432432432432435</v>
+        <v>1.5122873345935728</v>
       </c>
       <c r="C107">
-        <v>29.2</v>
+        <v>10.4</v>
       </c>
       <c r="D107">
         <v>1</v>
@@ -2913,13 +2889,13 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>65</v>
+        <v>157</v>
       </c>
       <c r="B108">
-        <v>1.5122873345935728</v>
+        <v>86.017554602980198</v>
       </c>
       <c r="C108">
-        <v>10.4</v>
+        <v>1</v>
       </c>
       <c r="D108">
         <v>1</v>
@@ -2931,13 +2907,13 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>157</v>
+        <v>66</v>
       </c>
       <c r="B109">
-        <v>86.017554602980198</v>
+        <v>100</v>
       </c>
       <c r="C109">
-        <v>1</v>
+        <v>8.6</v>
       </c>
       <c r="D109">
         <v>1</v>
@@ -2949,13 +2925,13 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B110">
-        <v>100</v>
+        <v>42.057291666666671</v>
       </c>
       <c r="C110">
-        <v>8.6</v>
+        <v>1</v>
       </c>
       <c r="D110">
         <v>1</v>
@@ -2967,13 +2943,13 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>67</v>
+        <v>130</v>
       </c>
       <c r="B111">
-        <v>42.057291666666671</v>
+        <v>100</v>
       </c>
       <c r="C111">
-        <v>1</v>
+        <v>19.5</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -2985,13 +2961,13 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>130</v>
+        <v>68</v>
       </c>
       <c r="B112">
-        <v>100</v>
+        <v>97.68518518518519</v>
       </c>
       <c r="C112">
-        <v>19.5</v>
+        <v>15.9</v>
       </c>
       <c r="D112">
         <v>1</v>
@@ -3003,13 +2979,13 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B113">
-        <v>97.68518518518519</v>
+        <v>97.353224254090478</v>
       </c>
       <c r="C113">
-        <v>15.9</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D113">
         <v>1</v>
@@ -3021,13 +2997,13 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B114">
-        <v>97.353224254090478</v>
+        <v>34.23180592991914</v>
       </c>
       <c r="C114">
-        <v>9.1999999999999993</v>
+        <v>3.6</v>
       </c>
       <c r="D114">
         <v>1</v>
@@ -3039,13 +3015,13 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B115">
-        <v>34.23180592991914</v>
+        <v>83.383534136546189</v>
       </c>
       <c r="C115">
-        <v>3.6</v>
+        <v>1</v>
       </c>
       <c r="D115">
         <v>1</v>
@@ -3057,13 +3033,13 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B116">
-        <v>83.383534136546189</v>
+        <v>99.740259740259745</v>
       </c>
       <c r="C116">
-        <v>1</v>
+        <v>6.3</v>
       </c>
       <c r="D116">
         <v>1</v>
@@ -3075,13 +3051,13 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B117">
-        <v>99.740259740259745</v>
+        <v>0.82057823129251706</v>
       </c>
       <c r="C117">
-        <v>6.3</v>
+        <v>14.9</v>
       </c>
       <c r="D117">
         <v>1</v>
@@ -3099,7 +3075,7 @@
         <v>0</v>
       </c>
       <c r="C118">
-        <v>14.9</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -3117,7 +3093,7 @@
         <v>0</v>
       </c>
       <c r="C119">
-        <v>9.8000000000000007</v>
+        <v>29.2</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -3129,13 +3105,13 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B120">
-        <v>0.82057823129251706</v>
+        <v>1</v>
       </c>
       <c r="C120">
-        <v>29.2</v>
+        <v>1</v>
       </c>
       <c r="D120">
         <v>1</v>
@@ -3147,13 +3123,13 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B121">
-        <v>1</v>
+        <v>88.257372654155503</v>
       </c>
       <c r="C121">
-        <v>1</v>
+        <v>8.5</v>
       </c>
       <c r="D121">
         <v>1</v>
@@ -3165,16 +3141,16 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>75</v>
+        <v>160</v>
       </c>
       <c r="B122">
-        <v>88.257372654155503</v>
+        <v>0</v>
       </c>
       <c r="C122">
-        <v>8.5</v>
+        <v>13.1</v>
       </c>
       <c r="D122">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E122">
         <v>1</v>
@@ -3183,16 +3159,16 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>160</v>
+        <v>76</v>
       </c>
       <c r="B123">
-        <v>0</v>
+        <v>6.3105835806132546</v>
       </c>
       <c r="C123">
-        <v>13.1</v>
+        <v>1</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E123">
         <v>1</v>
@@ -3201,16 +3177,16 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>76</v>
+        <v>161</v>
       </c>
       <c r="B124">
-        <v>6.3105835806132546</v>
+        <v>0</v>
       </c>
       <c r="C124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E124">
         <v>1</v>
@@ -3219,16 +3195,16 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>161</v>
+        <v>77</v>
       </c>
       <c r="B125">
-        <v>0</v>
+        <v>95.839598997493738</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E125">
         <v>1</v>
@@ -3237,10 +3213,10 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="B126">
-        <v>95.839598997493738</v>
+        <v>99.166550909848596</v>
       </c>
       <c r="C126">
         <v>1</v>
@@ -3255,13 +3231,13 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="B127">
-        <v>99.166550909848596</v>
+        <v>1</v>
       </c>
       <c r="C127">
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="D127">
         <v>1</v>
@@ -3273,13 +3249,13 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
-        <v>137</v>
+        <v>78</v>
       </c>
       <c r="B128">
         <v>1</v>
       </c>
       <c r="C128">
-        <v>12.5</v>
+        <v>1</v>
       </c>
       <c r="D128">
         <v>1</v>
@@ -3291,7 +3267,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -3309,13 +3285,13 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="B130">
-        <v>1</v>
+        <v>86.956521739130437</v>
       </c>
       <c r="C130">
-        <v>1</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="D130">
         <v>1</v>
@@ -3327,16 +3303,16 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="B131">
-        <v>86.956521739130437</v>
+        <v>0</v>
       </c>
       <c r="C131">
-        <v>35.700000000000003</v>
+        <v>6</v>
       </c>
       <c r="D131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E131">
         <v>1</v>
@@ -3345,13 +3321,13 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B132">
         <v>0</v>
       </c>
       <c r="C132">
-        <v>6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D132">
         <v>0</v>
@@ -3363,13 +3339,13 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B133">
         <v>0</v>
       </c>
       <c r="C133">
-        <v>4.0999999999999996</v>
+        <v>16.5</v>
       </c>
       <c r="D133">
         <v>0</v>
@@ -3381,16 +3357,16 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>164</v>
+        <v>80</v>
       </c>
       <c r="B134">
-        <v>0</v>
+        <v>58.846857840146427</v>
       </c>
       <c r="C134">
-        <v>16.5</v>
+        <v>7.8</v>
       </c>
       <c r="D134">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E134">
         <v>1</v>
@@ -3399,13 +3375,13 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="B135">
-        <v>58.846857840146427</v>
+        <v>100</v>
       </c>
       <c r="C135">
-        <v>7.8</v>
+        <v>10.9</v>
       </c>
       <c r="D135">
         <v>1</v>
@@ -3417,13 +3393,13 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="B136">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C136">
-        <v>10.9</v>
+        <v>1</v>
       </c>
       <c r="D136">
         <v>1</v>
@@ -3435,16 +3411,16 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="B137">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C137">
-        <v>1</v>
+        <v>3.8</v>
       </c>
       <c r="D137">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E137">
         <v>1</v>
@@ -3453,16 +3429,16 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>165</v>
+        <v>82</v>
       </c>
       <c r="B138">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C138">
-        <v>3.8</v>
+        <v>5.2</v>
       </c>
       <c r="D138">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E138">
         <v>1</v>
@@ -3471,13 +3447,13 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B139">
-        <v>1</v>
+        <v>54.464285714285708</v>
       </c>
       <c r="C139">
-        <v>5.2</v>
+        <v>1</v>
       </c>
       <c r="D139">
         <v>1</v>
@@ -3489,13 +3465,13 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B140">
-        <v>54.464285714285708</v>
+        <v>99.324324324324323</v>
       </c>
       <c r="C140">
-        <v>1</v>
+        <v>71.400000000000006</v>
       </c>
       <c r="D140">
         <v>1</v>
@@ -3507,13 +3483,13 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B141">
-        <v>99.324324324324323</v>
+        <v>51.941272430668839</v>
       </c>
       <c r="C141">
-        <v>71.400000000000006</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D141">
         <v>1</v>
@@ -3525,13 +3501,13 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B142">
-        <v>51.941272430668839</v>
+        <v>43.290414878397712</v>
       </c>
       <c r="C142">
-        <v>4.5999999999999996</v>
+        <v>1</v>
       </c>
       <c r="D142">
         <v>1</v>
@@ -3543,13 +3519,13 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>86</v>
+        <v>132</v>
       </c>
       <c r="B143">
-        <v>43.290414878397712</v>
+        <v>100</v>
       </c>
       <c r="C143">
-        <v>1</v>
+        <v>10.5</v>
       </c>
       <c r="D143">
         <v>1</v>
@@ -3561,16 +3537,16 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
       <c r="B144">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C144">
-        <v>10.5</v>
+        <v>7.9</v>
       </c>
       <c r="D144">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E144">
         <v>1</v>
@@ -3579,16 +3555,16 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>166</v>
+        <v>87</v>
       </c>
       <c r="B145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C145">
-        <v>7.9</v>
+        <v>1</v>
       </c>
       <c r="D145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E145">
         <v>1</v>
@@ -3597,10 +3573,10 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B146">
-        <v>1</v>
+        <v>56.333333333333336</v>
       </c>
       <c r="C146">
         <v>1</v>
@@ -3615,13 +3591,13 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B147">
-        <v>56.333333333333336</v>
+        <v>24.921364626179532</v>
       </c>
       <c r="C147">
-        <v>1</v>
+        <v>5.2</v>
       </c>
       <c r="D147">
         <v>1</v>
@@ -3633,13 +3609,13 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B148">
-        <v>24.921364626179532</v>
+        <v>46.559751681324371</v>
       </c>
       <c r="C148">
-        <v>5.2</v>
+        <v>24.9</v>
       </c>
       <c r="D148">
         <v>1</v>
@@ -3651,13 +3627,13 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B149">
-        <v>46.559751681324371</v>
+        <v>99.948875255623733</v>
       </c>
       <c r="C149">
-        <v>24.9</v>
+        <v>10.1</v>
       </c>
       <c r="D149">
         <v>1</v>
@@ -3669,16 +3645,16 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>91</v>
+        <v>167</v>
       </c>
       <c r="B150">
-        <v>99.948875255623733</v>
+        <v>0</v>
       </c>
       <c r="C150">
-        <v>10.1</v>
+        <v>20.3</v>
       </c>
       <c r="D150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E150">
         <v>1</v>
@@ -3687,16 +3663,16 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
       <c r="B151">
-        <v>0</v>
+        <v>92.715231788079464</v>
       </c>
       <c r="C151">
-        <v>20.3</v>
+        <v>8.1</v>
       </c>
       <c r="D151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E151">
         <v>1</v>
@@ -3705,13 +3681,13 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
       <c r="B152">
-        <v>92.715231788079464</v>
+        <v>75.513851653261838</v>
       </c>
       <c r="C152">
-        <v>8.1</v>
+        <v>3.7</v>
       </c>
       <c r="D152">
         <v>1</v>
@@ -3723,13 +3699,13 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B153">
-        <v>75.513851653261838</v>
+        <v>8.5270596987167568</v>
       </c>
       <c r="C153">
-        <v>3.7</v>
+        <v>1</v>
       </c>
       <c r="D153">
         <v>1</v>
@@ -3741,13 +3717,13 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="B154">
-        <v>8.5270596987167568</v>
+        <v>3.4640522875816995</v>
       </c>
       <c r="C154">
-        <v>1</v>
+        <v>4.5</v>
       </c>
       <c r="D154">
         <v>1</v>
@@ -3759,13 +3735,13 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B155">
-        <v>3.4640522875816995</v>
+        <v>94.609164420485172</v>
       </c>
       <c r="C155">
-        <v>4.5</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="D155">
         <v>1</v>
@@ -3777,13 +3753,13 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B156">
-        <v>94.609164420485172</v>
+        <v>1</v>
       </c>
       <c r="C156">
-        <v>20.399999999999999</v>
+        <v>1</v>
       </c>
       <c r="D156">
         <v>1</v>
@@ -3795,13 +3771,13 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B157">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C157">
-        <v>1</v>
+        <v>7.1</v>
       </c>
       <c r="D157">
         <v>1</v>
@@ -3813,13 +3789,13 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="B158">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C158">
-        <v>7.1</v>
+        <v>1</v>
       </c>
       <c r="D158">
         <v>1</v>
@@ -3831,13 +3807,13 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B159">
-        <v>1</v>
+        <v>94.45438282647585</v>
       </c>
       <c r="C159">
-        <v>1</v>
+        <v>24.1</v>
       </c>
       <c r="D159">
         <v>1</v>
@@ -3849,13 +3825,13 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B160">
-        <v>94.45438282647585</v>
+        <v>1</v>
       </c>
       <c r="C160">
-        <v>24.1</v>
+        <v>1</v>
       </c>
       <c r="D160">
         <v>1</v>
@@ -3867,7 +3843,7 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B161">
         <v>1</v>
@@ -3885,13 +3861,13 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B162">
-        <v>1</v>
+        <v>18.791380763211748</v>
       </c>
       <c r="C162">
-        <v>1</v>
+        <v>3.6</v>
       </c>
       <c r="D162">
         <v>1</v>
@@ -3903,13 +3879,13 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="B163">
-        <v>18.791380763211748</v>
+        <v>100</v>
       </c>
       <c r="C163">
-        <v>3.6</v>
+        <v>1</v>
       </c>
       <c r="D163">
         <v>1</v>
@@ -3921,13 +3897,13 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="B164">
-        <v>100</v>
+        <v>99.163179916317986</v>
       </c>
       <c r="C164">
-        <v>1</v>
+        <v>10.5</v>
       </c>
       <c r="D164">
         <v>1</v>
@@ -3939,13 +3915,13 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="B165">
-        <v>99.163179916317986</v>
+        <v>91.492776886035315</v>
       </c>
       <c r="C165">
-        <v>10.5</v>
+        <v>24.2</v>
       </c>
       <c r="D165">
         <v>1</v>
@@ -3957,13 +3933,13 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B166">
-        <v>91.492776886035315</v>
+        <v>1</v>
       </c>
       <c r="C166">
-        <v>24.2</v>
+        <v>42.7</v>
       </c>
       <c r="D166">
         <v>1</v>
@@ -3975,13 +3951,13 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B167">
-        <v>1</v>
+        <v>97.101449275362313</v>
       </c>
       <c r="C167">
-        <v>42.7</v>
+        <v>26.2</v>
       </c>
       <c r="D167">
         <v>1</v>
@@ -4000,12 +3976,6 @@
       </c>
       <c r="C168">
         <v>26.2</v>
-      </c>
-      <c r="D168">
-        <v>1</v>
-      </c>
-      <c r="E168">
-        <v>1</v>
       </c>
       <c r="G168" s="7"/>
     </row>

</xml_diff>

<commit_message>
Rewrite to py file
</commit_message>
<xml_diff>
--- a/data/figure-data.xlsx
+++ b/data/figure-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmor7802/repos/bivariate-map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92880A56-36E0-2649-8344-9BB9692B03F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDC2448-961E-3247-A4CE-BDB3D0E069AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{D0AE1AC3-FFDD-DB40-87A2-A3D733A83E2C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" tabRatio="500" xr2:uid="{D0AE1AC3-FFDD-DB40-87A2-A3D733A83E2C}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="9" r:id="rId1"/>
@@ -347,12 +347,6 @@
     <t>Country</t>
   </si>
   <si>
-    <t>Undernourishment</t>
-  </si>
-  <si>
-    <t>IDR</t>
-  </si>
-  <si>
     <t>no_IDR</t>
   </si>
   <si>
@@ -546,6 +540,12 @@
   </si>
   <si>
     <t>Chad</t>
+  </si>
+  <si>
+    <t>y_IDR</t>
+  </si>
+  <si>
+    <t>x_Undernourishment</t>
   </si>
 </sst>
 </file>
@@ -568,6 +568,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Display"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -954,7 +955,7 @@
   <dimension ref="A1:G205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -967,16 +968,16 @@
         <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1197,7 +1198,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1215,7 +1216,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1233,7 +1234,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B16">
         <v>61.501597444089462</v>
@@ -1251,7 +1252,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B17">
         <v>85.112936344969199</v>
@@ -1269,7 +1270,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B18">
         <v>70.314505776636722</v>
@@ -1323,7 +1324,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B21">
         <v>100</v>
@@ -1359,7 +1360,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B23">
         <v>100</v>
@@ -1413,7 +1414,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -1431,7 +1432,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B27">
         <v>100</v>
@@ -1449,7 +1450,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B28">
         <v>98.347107438016536</v>
@@ -1503,7 +1504,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B31">
         <v>97.945707997065298</v>
@@ -1539,7 +1540,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -1557,7 +1558,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B34">
         <v>100</v>
@@ -1575,7 +1576,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -1593,7 +1594,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B36">
         <v>100</v>
@@ -1629,7 +1630,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1683,7 +1684,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B41">
         <v>58.441558441558442</v>
@@ -1701,7 +1702,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B42">
         <v>98.469387755102048</v>
@@ -1737,7 +1738,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1755,7 +1756,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1773,7 +1774,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1791,7 +1792,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1845,7 +1846,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B50">
         <v>100</v>
@@ -1881,7 +1882,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B52">
         <v>100</v>
@@ -1917,7 +1918,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B54">
         <v>100</v>
@@ -1971,7 +1972,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -1989,7 +1990,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -2043,7 +2044,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -2097,7 +2098,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B64">
         <v>100</v>
@@ -2115,7 +2116,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -2133,7 +2134,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -2151,7 +2152,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B67">
         <v>100</v>
@@ -2187,7 +2188,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -2223,7 +2224,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -2259,7 +2260,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B73">
         <v>99.278474488919429</v>
@@ -2277,7 +2278,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B74">
         <v>11.556363636363637</v>
@@ -2367,7 +2368,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -2493,7 +2494,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -2655,7 +2656,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B95">
         <v>98.439450686641692</v>
@@ -2727,7 +2728,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -2889,7 +2890,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B108">
         <v>86.017554602980198</v>
@@ -2943,7 +2944,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B111">
         <v>100</v>
@@ -3069,7 +3070,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -3087,7 +3088,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -3141,7 +3142,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -3177,7 +3178,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -3213,7 +3214,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B126">
         <v>99.166550909848596</v>
@@ -3231,7 +3232,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -3267,7 +3268,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -3303,7 +3304,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -3321,7 +3322,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -3339,7 +3340,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B133">
         <v>0</v>
@@ -3375,7 +3376,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B135">
         <v>100</v>
@@ -3411,7 +3412,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -3519,7 +3520,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B143">
         <v>100</v>
@@ -3537,7 +3538,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -3645,7 +3646,7 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -3663,7 +3664,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B151">
         <v>92.715231788079464</v>
@@ -3699,7 +3700,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B153">
         <v>8.5270596987167568</v>
@@ -3789,7 +3790,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B158">
         <v>1</v>
@@ -3807,7 +3808,7 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B159">
         <v>94.45438282647585</v>
@@ -3879,7 +3880,7 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B163">
         <v>100</v>
@@ -3897,7 +3898,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B164">
         <v>99.163179916317986</v>

</xml_diff>